<commit_message>
Solucion de Problemas de Alpha 8= A8.1
Se arreglaron los siguientes problemas:

-Arreglado error en que los soldados no se activaban luego de enviar a tres soldados y quitar al primero.

-Arreglado error que guardaba el espacio en tropas de la mision cuando se envio, lo que no permitia enviar nuevos.

-Arreglado error en que las miones guardaban los objetos que estaban encima de ellas y al reaparecer no eran seleccionables
</commit_message>
<xml_diff>
--- a/Role of Kingdoms/Assets/Informacion en Excel/EnemigosInformacion.xlsx
+++ b/Role of Kingdoms/Assets/Informacion en Excel/EnemigosInformacion.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phantom Bullet\Documents\Role of Kingdoms (Demo V7.3)\Assets\Informacion en Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phantom Bullet\Documents\ROK\Role of Kingdoms\Assets\Informacion en Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="19200" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="19200" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -63,6 +63,39 @@
   </si>
   <si>
     <t>Oso_icono_enemigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//Debajo de esto se puede </t>
+  </si>
+  <si>
+    <t>//Poner todo lo que quiera</t>
+  </si>
+  <si>
+    <t>//Solo escriba la // siempre</t>
+  </si>
+  <si>
+    <t>//Aquí puede escribir</t>
+  </si>
+  <si>
+    <t>//Tambien</t>
+  </si>
+  <si>
+    <t>//Si lo hace</t>
+  </si>
+  <si>
+    <t>//toda esta hilera</t>
+  </si>
+  <si>
+    <t>//Y no ponga valores</t>
+  </si>
+  <si>
+    <t>//Saltados, siempre ponga todo</t>
+  </si>
+  <si>
+    <t>//rellene</t>
+  </si>
+  <si>
+    <t>//o dejelo vacio</t>
   </si>
 </sst>
 </file>
@@ -417,21 +450,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="34.140625" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +487,11 @@
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -476,8 +513,11 @@
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -499,8 +539,11 @@
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -523,51 +566,73 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="G16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Arreglo de Fallos y Agregacion de Detalle de A8.1 = A8.2
-Arreglado problema en que los soldados de la lista de mision desaparecian si se utilizaban las flechas y luego se arrastraban
(si estaban asignados a una mision)

-Modificado: Ahora solo puede hablar un soldado a la vez (Sonido de no poder enviar a mision)

-Arreglado: Ahora el sonido sigue activo aun cuando se oculta al soldado utilizando las flechas.
</commit_message>
<xml_diff>
--- a/Role of Kingdoms/Assets/Informacion en Excel/EnemigosInformacion.xlsx
+++ b/Role of Kingdoms/Assets/Informacion en Excel/EnemigosInformacion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="19200" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="6600" windowWidth="19200" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Arreglo de Errores y Modificacion = A8.8
-Agregacion de Misiones

-Arreglado error que pausaba el tiempo de creacion de soldados al pasar al mapa de misiones.

-Quitado desplegable que actuaba como intermediario para ver los tiempos de misiones
</commit_message>
<xml_diff>
--- a/Role of Kingdoms/Assets/Informacion en Excel/EnemigosInformacion.xlsx
+++ b/Role of Kingdoms/Assets/Informacion en Excel/EnemigosInformacion.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phantom Bullet\Documents\ROK\Role of Kingdoms\Assets\Informacion en Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hôgger\Desktop\Proyectos RoK Descargas\Role of Kingdoms 8.7\Assets\Informacion en Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6600" windowWidth="19200" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -44,36 +44,18 @@
     <t>Poderes</t>
   </si>
   <si>
-    <t>Araña Montañera</t>
-  </si>
-  <si>
     <t>Nombre Icono</t>
   </si>
   <si>
     <t>Araña_icono_enemigo</t>
   </si>
   <si>
-    <t>Cerdo Apestoso</t>
-  </si>
-  <si>
     <t>Cerdo_icono_enemigo</t>
   </si>
   <si>
-    <t>Oso Furioso</t>
-  </si>
-  <si>
     <t>Oso_icono_enemigo</t>
   </si>
   <si>
-    <t xml:space="preserve">//Debajo de esto se puede </t>
-  </si>
-  <si>
-    <t>//Poner todo lo que quiera</t>
-  </si>
-  <si>
-    <t>//Solo escriba la // siempre</t>
-  </si>
-  <si>
     <t>//Aquí puede escribir</t>
   </si>
   <si>
@@ -96,6 +78,69 @@
   </si>
   <si>
     <t>//o dejelo vacio</t>
+  </si>
+  <si>
+    <t>Oveja_icono_enemigo</t>
+  </si>
+  <si>
+    <t>//o dejelo vacio // 1 - 8</t>
+  </si>
+  <si>
+    <t>//o dejelo vacio // 1 - 11</t>
+  </si>
+  <si>
+    <t>//o dejelo vacio // 1 - 12</t>
+  </si>
+  <si>
+    <t>//o dejelo vacio // 1 - 9</t>
+  </si>
+  <si>
+    <t>Araña infecta</t>
+  </si>
+  <si>
+    <t>Araña roja</t>
+  </si>
+  <si>
+    <t>Araña cabezona</t>
+  </si>
+  <si>
+    <t>El señorito</t>
+  </si>
+  <si>
+    <t>Don jackie</t>
+  </si>
+  <si>
+    <t>Oveja dormilona</t>
+  </si>
+  <si>
+    <t>Oveja nerviosa</t>
+  </si>
+  <si>
+    <t>Oveja adulterada</t>
+  </si>
+  <si>
+    <t>Cerdo pastando</t>
+  </si>
+  <si>
+    <t>Cerdo vigilante</t>
+  </si>
+  <si>
+    <t>Cerdo infectado</t>
+  </si>
+  <si>
+    <t>El gran cerdo</t>
+  </si>
+  <si>
+    <t>Oso meloso</t>
+  </si>
+  <si>
+    <t>Oso invernando</t>
+  </si>
+  <si>
+    <t>Oso hambriento</t>
+  </si>
+  <si>
+    <t>Oso gigante</t>
   </si>
 </sst>
 </file>
@@ -229,23 +274,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -281,23 +309,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -450,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,50 +496,50 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -537,24 +548,24 @@
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -563,120 +574,479 @@
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>44</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>36</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>48</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>60</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>72</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>